<commit_message>
update yeu cau xu ly
</commit_message>
<xml_diff>
--- a/GENCO3/WorkFlowConfigStepScreen.xlsx
+++ b/GENCO3/WorkFlowConfigStepScreen.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>Chỉ đạo</t>
   </si>
@@ -56,13 +56,7 @@
     <t>Tham Gia</t>
   </si>
   <si>
-    <t>Review</t>
-  </si>
-  <si>
     <t>(checkbox)</t>
-  </si>
-  <si>
-    <t>(checkbox) + dropdown list</t>
   </si>
   <si>
     <t>Phòng ban (cùng phòng / khác phòng /tất cả)</t>
@@ -434,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -445,13 +439,12 @@
     <col min="1" max="1" width="17.875" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="1"/>
+    <col min="4" max="4" width="47.75" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="4" t="s">
         <v>7</v>
@@ -460,16 +453,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -477,19 +467,16 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -497,19 +484,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -517,19 +501,16 @@
         <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -537,19 +518,16 @@
         <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -557,19 +535,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
@@ -577,19 +552,16 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -597,16 +569,13 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>